<commit_message>
solved 4 ones problem
</commit_message>
<xml_diff>
--- a/Members.xlsx
+++ b/Members.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Desktop\Extra Curriculars\Fix N Clean\for APSC 100\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastasia\PycharmProjects\FIXNCLEAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E93D3FE-7D68-451E-886F-CC4121FDD577}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -101,13 +102,7 @@
     <t>Cleaning basement, dusting, COMPUTER HELP (printer setup I think), Shovelling based on weather</t>
   </si>
   <si>
-    <t>saturday afternoon</t>
-  </si>
-  <si>
     <t>furniture moved and floors vacuumed/cleaned. Likely some other shit</t>
-  </si>
-  <si>
-    <t>DRIVE SO TOLD HER SATURDAY MORNING ONLY</t>
   </si>
   <si>
     <t>Sectional couch removed from basement</t>
@@ -332,7 +327,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -768,32 +763,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="12" max="12" width="101.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="11" max="11" width="12.08984375" customWidth="1"/>
+    <col min="12" max="12" width="101.54296875" customWidth="1"/>
+    <col min="13" max="13" width="20.81640625" customWidth="1"/>
+    <col min="14" max="14" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="47" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -807,7 +802,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -837,18 +832,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -863,20 +858,20 @@
         <v>13</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -891,22 +886,22 @@
         <v>14</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -921,46 +916,48 @@
         <v>15</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -975,22 +972,22 @@
         <v>16</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1005,22 +1002,22 @@
         <v>17</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1035,20 +1032,20 @@
         <v>18</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1063,46 +1060,48 @@
         <v>19</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1117,20 +1116,20 @@
         <v>20</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1145,22 +1144,22 @@
         <v>21</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1177,16 +1176,16 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1201,20 +1200,20 @@
         <v>23</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1229,22 +1228,22 @@
         <v>24</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1257,53 +1256,53 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4"/>
@@ -1313,16 +1312,16 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1334,51 +1333,49 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="G20" s="3"/>
       <c r="H20" s="5"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1390,13 +1387,13 @@
       <c r="J21" s="4"/>
       <c r="K21" s="5"/>
       <c r="L21" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>